<commit_message>
commit. Added a new row
</commit_message>
<xml_diff>
--- a/Keyword_Framework_Flipkart/src/dataEngine/DataEngine.xlsx
+++ b/Keyword_Framework_Flipkart/src/dataEngine/DataEngine.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="6090" yWindow="3390" windowWidth="12810" windowHeight="8265" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="12810" windowHeight="8265" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="2" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="52">
   <si>
     <t>Description</t>
   </si>
@@ -575,10 +575,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -860,6 +860,23 @@
       </c>
       <c r="E16" t="s">
         <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>51</v>
+      </c>
+      <c r="B17" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17" t="s">
+        <v>17</v>
+      </c>
+      <c r="D17" t="s">
+        <v>39</v>
+      </c>
+      <c r="E17" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>